<commit_message>
update report payment excel new summary and add filed user
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22215" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21135" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ลำดับที่</t>
   </si>
@@ -59,13 +59,16 @@
   </si>
   <si>
     <t>รายงานการรับชำระเงินผ่าน POS</t>
+  </si>
+  <si>
+    <t>เจ้าหน้าที่รับชำระ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -151,6 +154,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,13 +459,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.25" customWidth="1"/>
     <col min="2" max="2" width="12.25" customWidth="1"/>
@@ -474,9 +480,10 @@
     <col min="11" max="11" width="13.375" customWidth="1"/>
     <col min="12" max="12" width="20.875" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25">
+    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -493,7 +500,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -504,21 +511,21 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1">
+    <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1">
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,16 +564,19 @@
       </c>
       <c r="M6" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="4.3307086614173231" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -579,7 +589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -591,7 +601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update template report cancel payment
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21135" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>เลขที่อ้างอิง</t>
   </si>
   <si>
-    <t>ยอดเงินก่อนภาษี</t>
-  </si>
-  <si>
     <t>ภาษีมูลค่าเพิ่ม</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>เจ้าหน้าที่รับชำระ</t>
+  </si>
+  <si>
+    <t>มูลค่าบริการ</t>
   </si>
 </sst>
 </file>
@@ -140,6 +140,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -151,12 +157,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -484,42 +484,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -554,19 +554,19 @@
         <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>14</v>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template report  payment and edit dropdown authorities
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="7395"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>หน่วยติดตามหนี้</t>
   </si>
   <si>
-    <t>เลขที่ใบแจ้งค่าบริการ/ชื่อบริการ</t>
-  </si>
-  <si>
     <t>ชำระโดย</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>มูลค่าบริการ</t>
+  </si>
+  <si>
+    <t>เลขที่ใบแจ้งค่าหนี้</t>
   </si>
 </sst>
 </file>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -545,28 +545,28 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all bug 20-05-18
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -4,15 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22470" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:L11"/>
 </workbook>
 </file>
 
@@ -462,7 +460,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -581,28 +579,4 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="4.3307086614173231" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
defect update report head hot 30/10/2018
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{948491F2-9D8C-4C61-A13A-AB03E0229841}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C4FA2C30-5D31-4B44-A3C4-E2B030305B86}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="5385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" customWidth="1"/>

</xml_diff>

<commit_message>
defect report and clearing and cancle
</commit_message>
<xml_diff>
--- a/src/main/webapp/report/excel/Payment-Report.xlsx
+++ b/src/main/webapp/report/excel/Payment-Report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FC328E27-12E7-405F-A4B5-E70DEDC868DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A2437465-0E5B-43E8-9327-A24E76009D63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="21405" windowHeight="5385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ลำดับที่</t>
   </si>
@@ -25,9 +25,6 @@
     <t>เลขที่ใบเสร็จ/ใบกำกับภาษี</t>
   </si>
   <si>
-    <t>เลขที่สัญญา</t>
-  </si>
-  <si>
     <t>ชื่อผู้ซื้อสินค้า/ผู้รับบริการ</t>
   </si>
   <si>
@@ -61,7 +58,16 @@
     <t>ประเภทบริการ</t>
   </si>
   <si>
-    <t>เจ้าหน้าที่รับชำระ (ชื่อ - นามสกุล)</t>
+    <t>เลขที่ลูกค้า</t>
+  </si>
+  <si>
+    <t>รหัสเจ้าหน้าที่รับชำระ</t>
+  </si>
+  <si>
+    <t>รหัสสถานที่รับขำระ</t>
+  </si>
+  <si>
+    <t>ชื่อสถานที่รับชำระ</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -144,6 +150,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N2"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,94 +528,106 @@
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.25">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+    <row r="1" spans="1:16" ht="20.25">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+    <row r="2" spans="1:16" ht="15.75">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
-    <row r="3" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+    <row r="3" spans="1:16" ht="17.25" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:16" ht="17.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:16" ht="17.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1">
+    <row r="6" spans="1:16" ht="15" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="3" t="s">
+      <c r="M7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +638,7 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K2:P2"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="4.3307086614173231" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>